<commit_message>
US15B Updated Code for Validation
</commit_message>
<xml_diff>
--- a/webapp/templates/GMIDSubmissionTemplate.xlsx
+++ b/webapp/templates/GMIDSubmissionTemplate.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\na20267\Desktop\BAM\HCI JOBS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\na20267\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6135"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10695" windowHeight="4050"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="448">
   <si>
     <t>Country</t>
   </si>
@@ -742,9 +742,6 @@
   </si>
   <si>
     <t>Channel</t>
-  </si>
-  <si>
-    <t>Requested By</t>
   </si>
   <si>
     <t>A</t>
@@ -1879,10 +1876,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1893,10 +1890,9 @@
     <col min="5" max="5" width="18.42578125" customWidth="1"/>
     <col min="6" max="7" width="18.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="21" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1920,9 +1916,6 @@
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -2071,23 +2064,23 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="16" t="s">
         <v>175</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G3" s="13">
         <v>0</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J3" s="8">
         <v>0</v>
@@ -2108,28 +2101,28 @@
         <v>217</v>
       </c>
       <c r="S3" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="T3" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="W3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="16" t="s">
         <v>176</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G4" s="14">
         <v>4</v>
@@ -2156,28 +2149,28 @@
         <v>218</v>
       </c>
       <c r="S4" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="T4" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="W4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="16" t="s">
         <v>177</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G5" s="15">
         <v>5</v>
@@ -2204,28 +2197,28 @@
         <v>219</v>
       </c>
       <c r="S5" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="T5" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="W5" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="16" t="s">
         <v>178</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="J6" s="4">
         <v>3</v>
@@ -2246,10 +2239,10 @@
         <v>220</v>
       </c>
       <c r="S6" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="T6" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
@@ -2257,20 +2250,20 @@
         <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="16" t="s">
         <v>179</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="S7" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="T7" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="T7" s="3" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="8" spans="1:23" ht="30" x14ac:dyDescent="0.25">
@@ -2278,14 +2271,14 @@
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="16" t="s">
         <v>180</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="9" spans="1:23" ht="30" x14ac:dyDescent="0.25">
@@ -2293,14 +2286,14 @@
         <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="16" t="s">
         <v>181</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
@@ -2308,14 +2301,14 @@
         <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="16" t="s">
         <v>182</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
@@ -2323,14 +2316,14 @@
         <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="16" t="s">
         <v>183</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
@@ -2338,14 +2331,14 @@
         <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="16" t="s">
         <v>184</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
@@ -2353,14 +2346,14 @@
         <v>14</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="16" t="s">
         <v>185</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -2368,14 +2361,14 @@
         <v>15</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="16" t="s">
         <v>186</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
@@ -2383,14 +2376,14 @@
         <v>16</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="16" t="s">
         <v>187</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
@@ -2398,14 +2391,14 @@
         <v>17</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="16" t="s">
         <v>188</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2413,14 +2406,14 @@
         <v>18</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="16" t="s">
         <v>189</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2428,14 +2421,14 @@
         <v>19</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="16" t="s">
         <v>190</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2443,14 +2436,14 @@
         <v>20</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="16" t="s">
         <v>191</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2458,14 +2451,14 @@
         <v>21</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="16" t="s">
         <v>192</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2473,14 +2466,14 @@
         <v>22</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="16" t="s">
         <v>193</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2488,14 +2481,14 @@
         <v>23</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="16" t="s">
         <v>194</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2503,14 +2496,14 @@
         <v>24</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="16" t="s">
         <v>140</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2518,14 +2511,14 @@
         <v>25</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="16" t="s">
         <v>196</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2533,14 +2526,14 @@
         <v>26</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="16" t="s">
         <v>197</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2548,14 +2541,14 @@
         <v>27</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="16" t="s">
         <v>198</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -2563,14 +2556,14 @@
         <v>28</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="16" t="s">
         <v>199</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2578,14 +2571,14 @@
         <v>29</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="16" t="s">
         <v>203</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2593,14 +2586,14 @@
         <v>30</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="16" t="s">
         <v>200</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2608,14 +2601,14 @@
         <v>31</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="16" t="s">
         <v>201</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -2623,14 +2616,14 @@
         <v>32</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="16" t="s">
         <v>202</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -2638,7 +2631,7 @@
         <v>33</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C32" s="1"/>
     </row>
@@ -2647,7 +2640,7 @@
         <v>34</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C33" s="1"/>
     </row>
@@ -2656,7 +2649,7 @@
         <v>35</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C34" s="1"/>
     </row>
@@ -2665,7 +2658,7 @@
         <v>36</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C35" s="1"/>
     </row>
@@ -2674,7 +2667,7 @@
         <v>37</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C36" s="1"/>
     </row>
@@ -2683,7 +2676,7 @@
         <v>38</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C37" s="1"/>
     </row>
@@ -2692,7 +2685,7 @@
         <v>39</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C38" s="1"/>
     </row>
@@ -2701,7 +2694,7 @@
         <v>40</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C39" s="1"/>
     </row>
@@ -2710,7 +2703,7 @@
         <v>41</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C40" s="1"/>
     </row>
@@ -2719,7 +2712,7 @@
         <v>42</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C41" s="1"/>
     </row>
@@ -2728,7 +2721,7 @@
         <v>43</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C42" s="1"/>
     </row>
@@ -2737,7 +2730,7 @@
         <v>44</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C43" s="1"/>
     </row>
@@ -2746,7 +2739,7 @@
         <v>45</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C44" s="1"/>
     </row>
@@ -2755,7 +2748,7 @@
         <v>46</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C45" s="1"/>
     </row>
@@ -2764,7 +2757,7 @@
         <v>47</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C46" s="1"/>
     </row>
@@ -2773,7 +2766,7 @@
         <v>48</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C47" s="1"/>
     </row>
@@ -2782,7 +2775,7 @@
         <v>49</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C48" s="1"/>
     </row>
@@ -2791,7 +2784,7 @@
         <v>50</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C49" s="1"/>
     </row>
@@ -2800,7 +2793,7 @@
         <v>51</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C50" s="1"/>
     </row>
@@ -2809,7 +2802,7 @@
         <v>52</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C51" s="1"/>
     </row>
@@ -2818,7 +2811,7 @@
         <v>53</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C52" s="1"/>
     </row>
@@ -2827,7 +2820,7 @@
         <v>54</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C53" s="1"/>
     </row>
@@ -2836,7 +2829,7 @@
         <v>55</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C54" s="1"/>
     </row>
@@ -2845,7 +2838,7 @@
         <v>56</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C55" s="1"/>
     </row>
@@ -2854,7 +2847,7 @@
         <v>57</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C56" s="1"/>
     </row>
@@ -2863,7 +2856,7 @@
         <v>58</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C57" s="1"/>
     </row>
@@ -2872,7 +2865,7 @@
         <v>59</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C58" s="1"/>
     </row>
@@ -2881,7 +2874,7 @@
         <v>60</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C59" s="1"/>
     </row>
@@ -2890,7 +2883,7 @@
         <v>61</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C60" s="1"/>
     </row>
@@ -2899,7 +2892,7 @@
         <v>62</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C61" s="1"/>
     </row>
@@ -2908,7 +2901,7 @@
         <v>63</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C62" s="1"/>
     </row>
@@ -2917,7 +2910,7 @@
         <v>64</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C63" s="1"/>
     </row>
@@ -2926,7 +2919,7 @@
         <v>65</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C64" s="1"/>
     </row>
@@ -2935,7 +2928,7 @@
         <v>66</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C65" s="1"/>
     </row>
@@ -2944,7 +2937,7 @@
         <v>67</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C66" s="1"/>
     </row>
@@ -2953,7 +2946,7 @@
         <v>68</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C67" s="1"/>
     </row>
@@ -2962,7 +2955,7 @@
         <v>69</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C68" s="1"/>
     </row>
@@ -2971,7 +2964,7 @@
         <v>70</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C69" s="1"/>
     </row>
@@ -2980,7 +2973,7 @@
         <v>71</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C70" s="1"/>
     </row>
@@ -2989,7 +2982,7 @@
         <v>72</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C71" s="1"/>
     </row>
@@ -2998,7 +2991,7 @@
         <v>73</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C72" s="1"/>
     </row>
@@ -3007,7 +3000,7 @@
         <v>74</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C73" s="1"/>
     </row>
@@ -3016,7 +3009,7 @@
         <v>75</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C74" s="1"/>
     </row>
@@ -3025,7 +3018,7 @@
         <v>76</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C75" s="1"/>
     </row>
@@ -3034,7 +3027,7 @@
         <v>77</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C76" s="1"/>
     </row>
@@ -3043,7 +3036,7 @@
         <v>78</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C77" s="1"/>
     </row>
@@ -3052,7 +3045,7 @@
         <v>79</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C78" s="1"/>
     </row>
@@ -3061,7 +3054,7 @@
         <v>80</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C79" s="1"/>
     </row>
@@ -3070,7 +3063,7 @@
         <v>81</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C80" s="1"/>
     </row>
@@ -3079,7 +3072,7 @@
         <v>82</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C81" s="1"/>
     </row>
@@ -3088,7 +3081,7 @@
         <v>83</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C82" s="1"/>
     </row>
@@ -3097,7 +3090,7 @@
         <v>84</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C83" s="1"/>
     </row>
@@ -3106,7 +3099,7 @@
         <v>85</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C84" s="1"/>
     </row>
@@ -3115,7 +3108,7 @@
         <v>86</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C85" s="1"/>
     </row>
@@ -3124,7 +3117,7 @@
         <v>87</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C86" s="1"/>
     </row>
@@ -3133,7 +3126,7 @@
         <v>88</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C87" s="1"/>
     </row>
@@ -3142,7 +3135,7 @@
         <v>89</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C88" s="1"/>
     </row>
@@ -3151,7 +3144,7 @@
         <v>91</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C89" s="1"/>
     </row>
@@ -3160,7 +3153,7 @@
         <v>92</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C90" s="1"/>
     </row>
@@ -3169,7 +3162,7 @@
         <v>93</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C91" s="1"/>
     </row>
@@ -3178,7 +3171,7 @@
         <v>94</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C92" s="1"/>
     </row>
@@ -3187,7 +3180,7 @@
         <v>95</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C93" s="1"/>
     </row>
@@ -3196,7 +3189,7 @@
         <v>96</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C94" s="1"/>
     </row>
@@ -3205,7 +3198,7 @@
         <v>97</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C95" s="1"/>
     </row>
@@ -3214,7 +3207,7 @@
         <v>98</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C96" s="1"/>
     </row>
@@ -3223,7 +3216,7 @@
         <v>99</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C97" s="1"/>
     </row>
@@ -3232,7 +3225,7 @@
         <v>100</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C98" s="1"/>
     </row>
@@ -3241,7 +3234,7 @@
         <v>101</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C99" s="1"/>
     </row>
@@ -3250,7 +3243,7 @@
         <v>102</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C100" s="1"/>
     </row>
@@ -3259,7 +3252,7 @@
         <v>103</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C101" s="1"/>
     </row>
@@ -3268,7 +3261,7 @@
         <v>104</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C102" s="1"/>
     </row>
@@ -3277,7 +3270,7 @@
         <v>105</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C103" s="1"/>
     </row>
@@ -3286,7 +3279,7 @@
         <v>106</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C104" s="1"/>
     </row>
@@ -3295,7 +3288,7 @@
         <v>107</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C105" s="1"/>
     </row>
@@ -3304,7 +3297,7 @@
         <v>108</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C106" s="1"/>
     </row>
@@ -3313,7 +3306,7 @@
         <v>109</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C107" s="1"/>
     </row>
@@ -3322,7 +3315,7 @@
         <v>110</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C108" s="1"/>
     </row>
@@ -3331,7 +3324,7 @@
         <v>111</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C109" s="1"/>
     </row>
@@ -3340,7 +3333,7 @@
         <v>112</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C110" s="1"/>
     </row>
@@ -3349,7 +3342,7 @@
         <v>113</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C111" s="1"/>
     </row>
@@ -3358,7 +3351,7 @@
         <v>114</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C112" s="1"/>
     </row>
@@ -3367,7 +3360,7 @@
         <v>115</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C113" s="1"/>
     </row>
@@ -3376,7 +3369,7 @@
         <v>116</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C114" s="1"/>
     </row>
@@ -3385,7 +3378,7 @@
         <v>117</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C115" s="1"/>
     </row>
@@ -3394,7 +3387,7 @@
         <v>118</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C116" s="1"/>
     </row>
@@ -3403,7 +3396,7 @@
         <v>119</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C117" s="1"/>
     </row>
@@ -3412,7 +3405,7 @@
         <v>120</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C118" s="1"/>
     </row>
@@ -3421,7 +3414,7 @@
         <v>121</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C119" s="1"/>
     </row>
@@ -3430,7 +3423,7 @@
         <v>122</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C120" s="1"/>
     </row>
@@ -3439,7 +3432,7 @@
         <v>123</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C121" s="1"/>
     </row>
@@ -3448,7 +3441,7 @@
         <v>124</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C122" s="1"/>
     </row>
@@ -3457,7 +3450,7 @@
         <v>125</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C123" s="1"/>
     </row>
@@ -3466,7 +3459,7 @@
         <v>126</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C124" s="1"/>
     </row>
@@ -3475,7 +3468,7 @@
         <v>127</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C125" s="1"/>
     </row>
@@ -3484,7 +3477,7 @@
         <v>128</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C126" s="1"/>
     </row>
@@ -3493,7 +3486,7 @@
         <v>129</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C127" s="1"/>
     </row>
@@ -3502,7 +3495,7 @@
         <v>130</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C128" s="1"/>
     </row>
@@ -3511,7 +3504,7 @@
         <v>131</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C129" s="1"/>
     </row>
@@ -3520,7 +3513,7 @@
         <v>132</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C130" s="1"/>
     </row>
@@ -3529,7 +3522,7 @@
         <v>133</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C131" s="1"/>
     </row>
@@ -3538,7 +3531,7 @@
         <v>134</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C132" s="1"/>
     </row>
@@ -3547,7 +3540,7 @@
         <v>135</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C133" s="1"/>
     </row>
@@ -3556,7 +3549,7 @@
         <v>136</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C134" s="1"/>
     </row>
@@ -3565,7 +3558,7 @@
         <v>137</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C135" s="1"/>
     </row>
@@ -3574,7 +3567,7 @@
         <v>138</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C136" s="1"/>
     </row>
@@ -3583,7 +3576,7 @@
         <v>139</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C137" s="1"/>
     </row>
@@ -3592,7 +3585,7 @@
         <v>140</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C138" s="1"/>
     </row>
@@ -3601,7 +3594,7 @@
         <v>141</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C139" s="1"/>
     </row>
@@ -3610,7 +3603,7 @@
         <v>142</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C140" s="1"/>
     </row>
@@ -3619,7 +3612,7 @@
         <v>143</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C141" s="1"/>
     </row>
@@ -3628,7 +3621,7 @@
         <v>144</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C142" s="1"/>
     </row>
@@ -3637,7 +3630,7 @@
         <v>145</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C143" s="1"/>
     </row>
@@ -3646,7 +3639,7 @@
         <v>146</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C144" s="1"/>
     </row>
@@ -3655,7 +3648,7 @@
         <v>147</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C145" s="1"/>
     </row>
@@ -3664,7 +3657,7 @@
         <v>148</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C146" s="1"/>
     </row>
@@ -3673,7 +3666,7 @@
         <v>149</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C147" s="1"/>
     </row>
@@ -3682,7 +3675,7 @@
         <v>150</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C148" s="1"/>
     </row>
@@ -3691,7 +3684,7 @@
         <v>151</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C149" s="1"/>
     </row>
@@ -3700,7 +3693,7 @@
         <v>152</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C150" s="1"/>
     </row>
@@ -3709,7 +3702,7 @@
         <v>153</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C151" s="1"/>
     </row>
@@ -3718,7 +3711,7 @@
         <v>154</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C152" s="1"/>
     </row>
@@ -3727,7 +3720,7 @@
         <v>155</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C153" s="1"/>
     </row>
@@ -3736,7 +3729,7 @@
         <v>156</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C154" s="1"/>
     </row>
@@ -3745,7 +3738,7 @@
         <v>157</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C155" s="1"/>
     </row>
@@ -3754,7 +3747,7 @@
         <v>158</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C156" s="1"/>
     </row>
@@ -3763,7 +3756,7 @@
         <v>159</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C157" s="1"/>
     </row>
@@ -3772,7 +3765,7 @@
         <v>160</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C158" s="1"/>
     </row>
@@ -3781,7 +3774,7 @@
         <v>161</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C159" s="1"/>
     </row>
@@ -3790,7 +3783,7 @@
         <v>162</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C160" s="1"/>
     </row>
@@ -3799,7 +3792,7 @@
         <v>163</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C161" s="1"/>
     </row>
@@ -3808,7 +3801,7 @@
         <v>164</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C162" s="1"/>
     </row>
@@ -3817,7 +3810,7 @@
         <v>165</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C163" s="1"/>
     </row>
@@ -3826,7 +3819,7 @@
         <v>166</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C164" s="1"/>
     </row>
@@ -3835,7 +3828,7 @@
         <v>167</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C165" s="1"/>
     </row>
@@ -3844,57 +3837,57 @@
         <v>168</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C166" s="1"/>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C167" s="1"/>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
@@ -3902,7 +3895,7 @@
         <v>169</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
@@ -3910,7 +3903,7 @@
         <v>170</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
@@ -3918,7 +3911,7 @@
         <v>171</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
@@ -3926,7 +3919,7 @@
         <v>172</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
@@ -3934,7 +3927,7 @@
         <v>90</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Excel Sheet. All countries now included and first row validation cleared.
</commit_message>
<xml_diff>
--- a/webapp/templates/GMIDSubmissionTemplate.xlsx
+++ b/webapp/templates/GMIDSubmissionTemplate.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\na20267\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://avanade-my.sharepoint.com/personal/richard_savenok_avanade_com/Documents/Dow/Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10695" windowHeight="4050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
-    <sheet name="DataSheet" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="DataSheet" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="Alert">DataSheet!$N$3:$N$6</definedName>
     <definedName name="Channel">DataSheet!$W$3:$W$5</definedName>
     <definedName name="Contry">Template!$A$7:$A$9</definedName>
-    <definedName name="Country">DataSheet!$B$3:$B$167</definedName>
+    <definedName name="Country">DataSheet!$B$3:$B$177</definedName>
     <definedName name="Currency">DataSheet!$E$3:$E$31</definedName>
     <definedName name="gmiddatabase.accdb_1" localSheetId="1" hidden="1">DataSheet!#REF!</definedName>
     <definedName name="Market">DataSheet!$H$3:$H$5</definedName>
@@ -1416,7 +1416,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1879,20 +1879,20 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="26.140625" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" customWidth="1"/>
-    <col min="4" max="4" width="33.140625" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="7" width="18.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" customWidth="1"/>
+    <col min="3" max="3" width="24.5546875" customWidth="1"/>
+    <col min="4" max="4" width="33.109375" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" customWidth="1"/>
+    <col min="6" max="7" width="18.44140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1919,26 +1919,27 @@
       </c>
     </row>
   </sheetData>
+  <dataConsolidate/>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576">
       <formula1>Currency</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
       <formula1>Country</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>Prod</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
       <formula1>Netting</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576">
       <formula1>Market</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
       <formula1>Quadrant</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576">
       <formula1>Channel</formula1>
     </dataValidation>
   </dataValidations>
@@ -1954,31 +1955,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W177"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B177"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="39.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="39.109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1"/>
-    <col min="8" max="8" width="36.42578125" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" customWidth="1"/>
+    <col min="8" max="8" width="36.44140625" customWidth="1"/>
     <col min="10" max="10" width="9" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" customWidth="1"/>
+    <col min="11" max="11" width="13.44140625" customWidth="1"/>
     <col min="13" max="13" width="9" customWidth="1"/>
-    <col min="14" max="14" width="32.5703125" customWidth="1"/>
+    <col min="14" max="14" width="32.5546875" customWidth="1"/>
     <col min="16" max="16" width="9" customWidth="1"/>
-    <col min="17" max="17" width="23.5703125" customWidth="1"/>
-    <col min="19" max="19" width="11.28515625" customWidth="1"/>
-    <col min="20" max="20" width="14.28515625" customWidth="1"/>
-    <col min="23" max="23" width="13.7109375" customWidth="1"/>
+    <col min="17" max="17" width="23.5546875" customWidth="1"/>
+    <col min="19" max="19" width="11.33203125" customWidth="1"/>
+    <col min="20" max="20" width="14.33203125" customWidth="1"/>
+    <col min="23" max="23" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -2012,7 +2013,7 @@
       </c>
       <c r="W1" s="18"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
@@ -2062,7 +2063,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>234</v>
       </c>
@@ -2110,7 +2111,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>235</v>
       </c>
@@ -2158,7 +2159,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>236</v>
       </c>
@@ -2206,7 +2207,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>237</v>
       </c>
@@ -2245,7 +2246,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -2266,7 +2267,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -2281,7 +2282,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -2296,7 +2297,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -2311,7 +2312,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -2326,7 +2327,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -2341,7 +2342,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -2356,7 +2357,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -2371,7 +2372,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -2386,7 +2387,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -2401,7 +2402,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -2416,7 +2417,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -2431,7 +2432,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -2446,7 +2447,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -2461,7 +2462,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -2476,7 +2477,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -2491,7 +2492,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -2506,7 +2507,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -2521,7 +2522,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
@@ -2536,7 +2537,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
@@ -2551,7 +2552,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>28</v>
       </c>
@@ -2566,7 +2567,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
@@ -2581,7 +2582,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
@@ -2596,7 +2597,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>31</v>
       </c>
@@ -2611,7 +2612,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>32</v>
       </c>
@@ -2626,7 +2627,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>33</v>
       </c>
@@ -2635,7 +2636,7 @@
       </c>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>34</v>
       </c>
@@ -2644,7 +2645,7 @@
       </c>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>35</v>
       </c>
@@ -2653,7 +2654,7 @@
       </c>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>36</v>
       </c>
@@ -2662,7 +2663,7 @@
       </c>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>37</v>
       </c>
@@ -2671,7 +2672,7 @@
       </c>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>38</v>
       </c>
@@ -2680,7 +2681,7 @@
       </c>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>39</v>
       </c>
@@ -2689,7 +2690,7 @@
       </c>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>40</v>
       </c>
@@ -2698,7 +2699,7 @@
       </c>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>41</v>
       </c>
@@ -2707,7 +2708,7 @@
       </c>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>42</v>
       </c>
@@ -2716,7 +2717,7 @@
       </c>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>43</v>
       </c>
@@ -2725,7 +2726,7 @@
       </c>
       <c r="C42" s="1"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>44</v>
       </c>
@@ -2734,7 +2735,7 @@
       </c>
       <c r="C43" s="1"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>45</v>
       </c>
@@ -2743,7 +2744,7 @@
       </c>
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>46</v>
       </c>
@@ -2752,7 +2753,7 @@
       </c>
       <c r="C45" s="1"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>47</v>
       </c>
@@ -2761,7 +2762,7 @@
       </c>
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>48</v>
       </c>
@@ -2770,7 +2771,7 @@
       </c>
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>49</v>
       </c>
@@ -2779,7 +2780,7 @@
       </c>
       <c r="C48" s="1"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>50</v>
       </c>
@@ -2788,7 +2789,7 @@
       </c>
       <c r="C49" s="1"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>51</v>
       </c>
@@ -2797,7 +2798,7 @@
       </c>
       <c r="C50" s="1"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>52</v>
       </c>
@@ -2806,7 +2807,7 @@
       </c>
       <c r="C51" s="1"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>53</v>
       </c>
@@ -2815,7 +2816,7 @@
       </c>
       <c r="C52" s="1"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>54</v>
       </c>
@@ -2824,7 +2825,7 @@
       </c>
       <c r="C53" s="1"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>55</v>
       </c>
@@ -2833,7 +2834,7 @@
       </c>
       <c r="C54" s="1"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>56</v>
       </c>
@@ -2842,7 +2843,7 @@
       </c>
       <c r="C55" s="1"/>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>57</v>
       </c>
@@ -2851,7 +2852,7 @@
       </c>
       <c r="C56" s="1"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>58</v>
       </c>
@@ -2860,7 +2861,7 @@
       </c>
       <c r="C57" s="1"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>59</v>
       </c>
@@ -2869,7 +2870,7 @@
       </c>
       <c r="C58" s="1"/>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>60</v>
       </c>
@@ -2878,7 +2879,7 @@
       </c>
       <c r="C59" s="1"/>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>61</v>
       </c>
@@ -2887,7 +2888,7 @@
       </c>
       <c r="C60" s="1"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>62</v>
       </c>
@@ -2896,7 +2897,7 @@
       </c>
       <c r="C61" s="1"/>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>63</v>
       </c>
@@ -2905,7 +2906,7 @@
       </c>
       <c r="C62" s="1"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>64</v>
       </c>
@@ -2914,7 +2915,7 @@
       </c>
       <c r="C63" s="1"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>65</v>
       </c>
@@ -2923,7 +2924,7 @@
       </c>
       <c r="C64" s="1"/>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>66</v>
       </c>
@@ -2932,7 +2933,7 @@
       </c>
       <c r="C65" s="1"/>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>67</v>
       </c>
@@ -2941,7 +2942,7 @@
       </c>
       <c r="C66" s="1"/>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>68</v>
       </c>
@@ -2950,7 +2951,7 @@
       </c>
       <c r="C67" s="1"/>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>69</v>
       </c>
@@ -2959,7 +2960,7 @@
       </c>
       <c r="C68" s="1"/>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>70</v>
       </c>
@@ -2968,7 +2969,7 @@
       </c>
       <c r="C69" s="1"/>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>71</v>
       </c>
@@ -2977,7 +2978,7 @@
       </c>
       <c r="C70" s="1"/>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>72</v>
       </c>
@@ -2986,7 +2987,7 @@
       </c>
       <c r="C71" s="1"/>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>73</v>
       </c>
@@ -2995,7 +2996,7 @@
       </c>
       <c r="C72" s="1"/>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>74</v>
       </c>
@@ -3004,7 +3005,7 @@
       </c>
       <c r="C73" s="1"/>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>75</v>
       </c>
@@ -3013,7 +3014,7 @@
       </c>
       <c r="C74" s="1"/>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>76</v>
       </c>
@@ -3022,7 +3023,7 @@
       </c>
       <c r="C75" s="1"/>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>77</v>
       </c>
@@ -3031,7 +3032,7 @@
       </c>
       <c r="C76" s="1"/>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>78</v>
       </c>
@@ -3040,7 +3041,7 @@
       </c>
       <c r="C77" s="1"/>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>79</v>
       </c>
@@ -3049,7 +3050,7 @@
       </c>
       <c r="C78" s="1"/>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>80</v>
       </c>
@@ -3058,7 +3059,7 @@
       </c>
       <c r="C79" s="1"/>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>81</v>
       </c>
@@ -3067,7 +3068,7 @@
       </c>
       <c r="C80" s="1"/>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>82</v>
       </c>
@@ -3076,7 +3077,7 @@
       </c>
       <c r="C81" s="1"/>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>83</v>
       </c>
@@ -3085,7 +3086,7 @@
       </c>
       <c r="C82" s="1"/>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>84</v>
       </c>
@@ -3094,7 +3095,7 @@
       </c>
       <c r="C83" s="1"/>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>85</v>
       </c>
@@ -3103,7 +3104,7 @@
       </c>
       <c r="C84" s="1"/>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>86</v>
       </c>
@@ -3112,7 +3113,7 @@
       </c>
       <c r="C85" s="1"/>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>87</v>
       </c>
@@ -3121,7 +3122,7 @@
       </c>
       <c r="C86" s="1"/>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>88</v>
       </c>
@@ -3130,7 +3131,7 @@
       </c>
       <c r="C87" s="1"/>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>89</v>
       </c>
@@ -3139,7 +3140,7 @@
       </c>
       <c r="C88" s="1"/>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>91</v>
       </c>
@@ -3148,7 +3149,7 @@
       </c>
       <c r="C89" s="1"/>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>92</v>
       </c>
@@ -3157,7 +3158,7 @@
       </c>
       <c r="C90" s="1"/>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>93</v>
       </c>
@@ -3166,7 +3167,7 @@
       </c>
       <c r="C91" s="1"/>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>94</v>
       </c>
@@ -3175,7 +3176,7 @@
       </c>
       <c r="C92" s="1"/>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>95</v>
       </c>
@@ -3184,7 +3185,7 @@
       </c>
       <c r="C93" s="1"/>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>96</v>
       </c>
@@ -3193,7 +3194,7 @@
       </c>
       <c r="C94" s="1"/>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>97</v>
       </c>
@@ -3202,7 +3203,7 @@
       </c>
       <c r="C95" s="1"/>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>98</v>
       </c>
@@ -3211,7 +3212,7 @@
       </c>
       <c r="C96" s="1"/>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>99</v>
       </c>
@@ -3220,7 +3221,7 @@
       </c>
       <c r="C97" s="1"/>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>100</v>
       </c>
@@ -3229,7 +3230,7 @@
       </c>
       <c r="C98" s="1"/>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>101</v>
       </c>
@@ -3238,7 +3239,7 @@
       </c>
       <c r="C99" s="1"/>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>102</v>
       </c>
@@ -3247,7 +3248,7 @@
       </c>
       <c r="C100" s="1"/>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>103</v>
       </c>
@@ -3256,7 +3257,7 @@
       </c>
       <c r="C101" s="1"/>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>104</v>
       </c>
@@ -3265,7 +3266,7 @@
       </c>
       <c r="C102" s="1"/>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>105</v>
       </c>
@@ -3274,7 +3275,7 @@
       </c>
       <c r="C103" s="1"/>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>106</v>
       </c>
@@ -3283,7 +3284,7 @@
       </c>
       <c r="C104" s="1"/>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>107</v>
       </c>
@@ -3292,7 +3293,7 @@
       </c>
       <c r="C105" s="1"/>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>108</v>
       </c>
@@ -3301,7 +3302,7 @@
       </c>
       <c r="C106" s="1"/>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>109</v>
       </c>
@@ -3310,7 +3311,7 @@
       </c>
       <c r="C107" s="1"/>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>110</v>
       </c>
@@ -3319,7 +3320,7 @@
       </c>
       <c r="C108" s="1"/>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>111</v>
       </c>
@@ -3328,7 +3329,7 @@
       </c>
       <c r="C109" s="1"/>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>112</v>
       </c>
@@ -3337,7 +3338,7 @@
       </c>
       <c r="C110" s="1"/>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>113</v>
       </c>
@@ -3346,7 +3347,7 @@
       </c>
       <c r="C111" s="1"/>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>114</v>
       </c>
@@ -3355,7 +3356,7 @@
       </c>
       <c r="C112" s="1"/>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>115</v>
       </c>
@@ -3364,7 +3365,7 @@
       </c>
       <c r="C113" s="1"/>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>116</v>
       </c>
@@ -3373,7 +3374,7 @@
       </c>
       <c r="C114" s="1"/>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>117</v>
       </c>
@@ -3382,7 +3383,7 @@
       </c>
       <c r="C115" s="1"/>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>118</v>
       </c>
@@ -3391,7 +3392,7 @@
       </c>
       <c r="C116" s="1"/>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>119</v>
       </c>
@@ -3400,7 +3401,7 @@
       </c>
       <c r="C117" s="1"/>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>120</v>
       </c>
@@ -3409,7 +3410,7 @@
       </c>
       <c r="C118" s="1"/>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>121</v>
       </c>
@@ -3418,7 +3419,7 @@
       </c>
       <c r="C119" s="1"/>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>122</v>
       </c>
@@ -3427,7 +3428,7 @@
       </c>
       <c r="C120" s="1"/>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>123</v>
       </c>
@@ -3436,7 +3437,7 @@
       </c>
       <c r="C121" s="1"/>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>124</v>
       </c>
@@ -3445,7 +3446,7 @@
       </c>
       <c r="C122" s="1"/>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>125</v>
       </c>
@@ -3454,7 +3455,7 @@
       </c>
       <c r="C123" s="1"/>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>126</v>
       </c>
@@ -3463,7 +3464,7 @@
       </c>
       <c r="C124" s="1"/>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>127</v>
       </c>
@@ -3472,7 +3473,7 @@
       </c>
       <c r="C125" s="1"/>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>128</v>
       </c>
@@ -3481,7 +3482,7 @@
       </c>
       <c r="C126" s="1"/>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>129</v>
       </c>
@@ -3490,7 +3491,7 @@
       </c>
       <c r="C127" s="1"/>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>130</v>
       </c>
@@ -3499,7 +3500,7 @@
       </c>
       <c r="C128" s="1"/>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>131</v>
       </c>
@@ -3508,7 +3509,7 @@
       </c>
       <c r="C129" s="1"/>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>132</v>
       </c>
@@ -3517,7 +3518,7 @@
       </c>
       <c r="C130" s="1"/>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>133</v>
       </c>
@@ -3526,7 +3527,7 @@
       </c>
       <c r="C131" s="1"/>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>134</v>
       </c>
@@ -3535,7 +3536,7 @@
       </c>
       <c r="C132" s="1"/>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>135</v>
       </c>
@@ -3544,7 +3545,7 @@
       </c>
       <c r="C133" s="1"/>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>136</v>
       </c>
@@ -3553,7 +3554,7 @@
       </c>
       <c r="C134" s="1"/>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
         <v>137</v>
       </c>
@@ -3562,7 +3563,7 @@
       </c>
       <c r="C135" s="1"/>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>138</v>
       </c>
@@ -3571,7 +3572,7 @@
       </c>
       <c r="C136" s="1"/>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>139</v>
       </c>
@@ -3580,7 +3581,7 @@
       </c>
       <c r="C137" s="1"/>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
         <v>140</v>
       </c>
@@ -3589,7 +3590,7 @@
       </c>
       <c r="C138" s="1"/>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>141</v>
       </c>
@@ -3598,7 +3599,7 @@
       </c>
       <c r="C139" s="1"/>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>142</v>
       </c>
@@ -3607,7 +3608,7 @@
       </c>
       <c r="C140" s="1"/>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
         <v>143</v>
       </c>
@@ -3616,7 +3617,7 @@
       </c>
       <c r="C141" s="1"/>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>144</v>
       </c>
@@ -3625,7 +3626,7 @@
       </c>
       <c r="C142" s="1"/>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>145</v>
       </c>
@@ -3634,7 +3635,7 @@
       </c>
       <c r="C143" s="1"/>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>146</v>
       </c>
@@ -3643,7 +3644,7 @@
       </c>
       <c r="C144" s="1"/>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>147</v>
       </c>
@@ -3652,7 +3653,7 @@
       </c>
       <c r="C145" s="1"/>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>148</v>
       </c>
@@ -3661,7 +3662,7 @@
       </c>
       <c r="C146" s="1"/>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
         <v>149</v>
       </c>
@@ -3670,7 +3671,7 @@
       </c>
       <c r="C147" s="1"/>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>150</v>
       </c>
@@ -3679,7 +3680,7 @@
       </c>
       <c r="C148" s="1"/>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
         <v>151</v>
       </c>
@@ -3688,7 +3689,7 @@
       </c>
       <c r="C149" s="1"/>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>152</v>
       </c>
@@ -3697,7 +3698,7 @@
       </c>
       <c r="C150" s="1"/>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
         <v>153</v>
       </c>
@@ -3706,7 +3707,7 @@
       </c>
       <c r="C151" s="1"/>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
         <v>154</v>
       </c>
@@ -3715,7 +3716,7 @@
       </c>
       <c r="C152" s="1"/>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
         <v>155</v>
       </c>
@@ -3724,7 +3725,7 @@
       </c>
       <c r="C153" s="1"/>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>156</v>
       </c>
@@ -3733,7 +3734,7 @@
       </c>
       <c r="C154" s="1"/>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
         <v>157</v>
       </c>
@@ -3742,7 +3743,7 @@
       </c>
       <c r="C155" s="1"/>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>158</v>
       </c>
@@ -3751,7 +3752,7 @@
       </c>
       <c r="C156" s="1"/>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>159</v>
       </c>
@@ -3760,7 +3761,7 @@
       </c>
       <c r="C157" s="1"/>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>160</v>
       </c>
@@ -3769,7 +3770,7 @@
       </c>
       <c r="C158" s="1"/>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>161</v>
       </c>
@@ -3778,7 +3779,7 @@
       </c>
       <c r="C159" s="1"/>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>162</v>
       </c>
@@ -3787,7 +3788,7 @@
       </c>
       <c r="C160" s="1"/>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
         <v>163</v>
       </c>
@@ -3796,7 +3797,7 @@
       </c>
       <c r="C161" s="1"/>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>164</v>
       </c>
@@ -3805,7 +3806,7 @@
       </c>
       <c r="C162" s="1"/>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
         <v>165</v>
       </c>
@@ -3814,7 +3815,7 @@
       </c>
       <c r="C163" s="1"/>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
         <v>166</v>
       </c>
@@ -3823,7 +3824,7 @@
       </c>
       <c r="C164" s="1"/>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
         <v>167</v>
       </c>
@@ -3832,7 +3833,7 @@
       </c>
       <c r="C165" s="1"/>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
         <v>168</v>
       </c>
@@ -3841,7 +3842,7 @@
       </c>
       <c r="C166" s="1"/>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
         <v>238</v>
       </c>
@@ -3850,7 +3851,7 @@
       </c>
       <c r="C167" s="1"/>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>239</v>
       </c>
@@ -3858,7 +3859,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
         <v>240</v>
       </c>
@@ -3866,7 +3867,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
         <v>241</v>
       </c>
@@ -3874,7 +3875,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
         <v>242</v>
       </c>
@@ -3882,7 +3883,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
         <v>243</v>
       </c>
@@ -3890,7 +3891,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
         <v>169</v>
       </c>
@@ -3898,7 +3899,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
         <v>170</v>
       </c>
@@ -3906,7 +3907,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
         <v>171</v>
       </c>
@@ -3914,7 +3915,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
         <v>172</v>
       </c>
@@ -3922,7 +3923,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
         <v>90</v>
       </c>

</xml_diff>

<commit_message>
BAM.2017.S7.US27A, merge down from development to local branch BAM.2017.S7.US30B, QA issue - fixed security for checkbox on gmid submission page
</commit_message>
<xml_diff>
--- a/webapp/templates/GMIDSubmissionTemplate.xlsx
+++ b/webapp/templates/GMIDSubmissionTemplate.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\na20267\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://avanade-my.sharepoint.com/personal/richard_savenok_avanade_com/Documents/Dow/Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10695" windowHeight="4050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -19,11 +19,11 @@
     <definedName name="Alert">DataSheet!$N$3:$N$6</definedName>
     <definedName name="Channel">DataSheet!$W$3:$W$5</definedName>
     <definedName name="Contry">Template!$A$7:$A$9</definedName>
-    <definedName name="Country">DataSheet!$B$3:$B$167</definedName>
+    <definedName name="Country">DataSheet!$B$3:$B$177</definedName>
     <definedName name="Currency">DataSheet!$E$3:$E$31</definedName>
     <definedName name="gmiddatabase.accdb_1" localSheetId="1" hidden="1">DataSheet!#REF!</definedName>
     <definedName name="Market">DataSheet!$H$3:$H$5</definedName>
-    <definedName name="Netting">DataSheet!$K$3:$K$6</definedName>
+    <definedName name="Netting">DataSheet!$K$3:$K$7</definedName>
     <definedName name="Prod">DataSheet!$Q$3:$Q$6</definedName>
     <definedName name="Quadrant">DataSheet!$T$3:$T$7</definedName>
     <definedName name="test">Template!$A$7:$A$9</definedName>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="449">
   <si>
     <t>Country</t>
   </si>
@@ -1411,12 +1411,15 @@
   </si>
   <si>
     <t>ZAR - South African Rand</t>
+  </si>
+  <si>
+    <t>5 - Crop Constrained</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1878,21 +1881,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="26.140625" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" customWidth="1"/>
-    <col min="4" max="4" width="33.140625" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="7" width="18.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" customWidth="1"/>
+    <col min="3" max="3" width="24.5546875" customWidth="1"/>
+    <col min="4" max="4" width="33.109375" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" customWidth="1"/>
+    <col min="6" max="7" width="18.44140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1919,26 +1920,27 @@
       </c>
     </row>
   </sheetData>
+  <dataConsolidate/>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576">
       <formula1>Currency</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
       <formula1>Country</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>Prod</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
       <formula1>Netting</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576">
       <formula1>Market</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
       <formula1>Quadrant</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576">
       <formula1>Channel</formula1>
     </dataValidation>
   </dataValidations>
@@ -1954,31 +1956,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W177"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3:K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="39.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="39.109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1"/>
-    <col min="8" max="8" width="36.42578125" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" customWidth="1"/>
+    <col min="8" max="8" width="36.44140625" customWidth="1"/>
     <col min="10" max="10" width="9" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" customWidth="1"/>
+    <col min="11" max="11" width="13.44140625" customWidth="1"/>
     <col min="13" max="13" width="9" customWidth="1"/>
-    <col min="14" max="14" width="32.5703125" customWidth="1"/>
+    <col min="14" max="14" width="32.5546875" customWidth="1"/>
     <col min="16" max="16" width="9" customWidth="1"/>
-    <col min="17" max="17" width="23.5703125" customWidth="1"/>
-    <col min="19" max="19" width="11.28515625" customWidth="1"/>
-    <col min="20" max="20" width="14.28515625" customWidth="1"/>
-    <col min="23" max="23" width="13.7109375" customWidth="1"/>
+    <col min="17" max="17" width="23.5546875" customWidth="1"/>
+    <col min="19" max="19" width="11.33203125" customWidth="1"/>
+    <col min="20" max="20" width="14.33203125" customWidth="1"/>
+    <col min="23" max="23" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -2012,7 +2014,7 @@
       </c>
       <c r="W1" s="18"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
@@ -2062,7 +2064,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>234</v>
       </c>
@@ -2110,7 +2112,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>235</v>
       </c>
@@ -2158,7 +2160,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>236</v>
       </c>
@@ -2206,7 +2208,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>237</v>
       </c>
@@ -2245,7 +2247,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -2259,6 +2261,12 @@
       <c r="E7" s="16" t="s">
         <v>423</v>
       </c>
+      <c r="J7" s="8">
+        <v>5</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>448</v>
+      </c>
       <c r="S7" s="2" t="s">
         <v>229</v>
       </c>
@@ -2266,7 +2274,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -2280,8 +2288,9 @@
       <c r="E8" s="16" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="9" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -2296,7 +2305,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -2311,7 +2320,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -2326,7 +2335,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -2341,7 +2350,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -2356,7 +2365,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -2371,7 +2380,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -2386,7 +2395,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -2401,7 +2410,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -2416,7 +2425,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -2431,7 +2440,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -2446,7 +2455,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -2461,7 +2470,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -2476,7 +2485,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -2491,7 +2500,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -2506,7 +2515,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -2521,7 +2530,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
@@ -2536,7 +2545,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
@@ -2551,7 +2560,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>28</v>
       </c>
@@ -2566,7 +2575,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
@@ -2581,7 +2590,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
@@ -2596,7 +2605,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>31</v>
       </c>
@@ -2611,7 +2620,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>32</v>
       </c>
@@ -2626,7 +2635,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>33</v>
       </c>
@@ -2635,7 +2644,7 @@
       </c>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>34</v>
       </c>
@@ -2644,7 +2653,7 @@
       </c>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>35</v>
       </c>
@@ -2653,7 +2662,7 @@
       </c>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>36</v>
       </c>
@@ -2662,7 +2671,7 @@
       </c>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>37</v>
       </c>
@@ -2671,7 +2680,7 @@
       </c>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>38</v>
       </c>
@@ -2680,7 +2689,7 @@
       </c>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>39</v>
       </c>
@@ -2689,7 +2698,7 @@
       </c>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>40</v>
       </c>
@@ -2698,7 +2707,7 @@
       </c>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>41</v>
       </c>
@@ -2707,7 +2716,7 @@
       </c>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>42</v>
       </c>
@@ -2716,7 +2725,7 @@
       </c>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>43</v>
       </c>
@@ -2725,7 +2734,7 @@
       </c>
       <c r="C42" s="1"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>44</v>
       </c>
@@ -2734,7 +2743,7 @@
       </c>
       <c r="C43" s="1"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>45</v>
       </c>
@@ -2743,7 +2752,7 @@
       </c>
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>46</v>
       </c>
@@ -2752,7 +2761,7 @@
       </c>
       <c r="C45" s="1"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>47</v>
       </c>
@@ -2761,7 +2770,7 @@
       </c>
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>48</v>
       </c>
@@ -2770,7 +2779,7 @@
       </c>
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>49</v>
       </c>
@@ -2779,7 +2788,7 @@
       </c>
       <c r="C48" s="1"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>50</v>
       </c>
@@ -2788,7 +2797,7 @@
       </c>
       <c r="C49" s="1"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>51</v>
       </c>
@@ -2797,7 +2806,7 @@
       </c>
       <c r="C50" s="1"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>52</v>
       </c>
@@ -2806,7 +2815,7 @@
       </c>
       <c r="C51" s="1"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>53</v>
       </c>
@@ -2815,7 +2824,7 @@
       </c>
       <c r="C52" s="1"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>54</v>
       </c>
@@ -2824,7 +2833,7 @@
       </c>
       <c r="C53" s="1"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>55</v>
       </c>
@@ -2833,7 +2842,7 @@
       </c>
       <c r="C54" s="1"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>56</v>
       </c>
@@ -2842,7 +2851,7 @@
       </c>
       <c r="C55" s="1"/>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>57</v>
       </c>
@@ -2851,7 +2860,7 @@
       </c>
       <c r="C56" s="1"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>58</v>
       </c>
@@ -2860,7 +2869,7 @@
       </c>
       <c r="C57" s="1"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>59</v>
       </c>
@@ -2869,7 +2878,7 @@
       </c>
       <c r="C58" s="1"/>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>60</v>
       </c>
@@ -2878,7 +2887,7 @@
       </c>
       <c r="C59" s="1"/>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>61</v>
       </c>
@@ -2887,7 +2896,7 @@
       </c>
       <c r="C60" s="1"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>62</v>
       </c>
@@ -2896,7 +2905,7 @@
       </c>
       <c r="C61" s="1"/>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>63</v>
       </c>
@@ -2905,7 +2914,7 @@
       </c>
       <c r="C62" s="1"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>64</v>
       </c>
@@ -2914,7 +2923,7 @@
       </c>
       <c r="C63" s="1"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>65</v>
       </c>
@@ -2923,7 +2932,7 @@
       </c>
       <c r="C64" s="1"/>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>66</v>
       </c>
@@ -2932,7 +2941,7 @@
       </c>
       <c r="C65" s="1"/>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>67</v>
       </c>
@@ -2941,7 +2950,7 @@
       </c>
       <c r="C66" s="1"/>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>68</v>
       </c>
@@ -2950,7 +2959,7 @@
       </c>
       <c r="C67" s="1"/>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>69</v>
       </c>
@@ -2959,7 +2968,7 @@
       </c>
       <c r="C68" s="1"/>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>70</v>
       </c>
@@ -2968,7 +2977,7 @@
       </c>
       <c r="C69" s="1"/>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>71</v>
       </c>
@@ -2977,7 +2986,7 @@
       </c>
       <c r="C70" s="1"/>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>72</v>
       </c>
@@ -2986,7 +2995,7 @@
       </c>
       <c r="C71" s="1"/>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>73</v>
       </c>
@@ -2995,7 +3004,7 @@
       </c>
       <c r="C72" s="1"/>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>74</v>
       </c>
@@ -3004,7 +3013,7 @@
       </c>
       <c r="C73" s="1"/>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>75</v>
       </c>
@@ -3013,7 +3022,7 @@
       </c>
       <c r="C74" s="1"/>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>76</v>
       </c>
@@ -3022,7 +3031,7 @@
       </c>
       <c r="C75" s="1"/>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>77</v>
       </c>
@@ -3031,7 +3040,7 @@
       </c>
       <c r="C76" s="1"/>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>78</v>
       </c>
@@ -3040,7 +3049,7 @@
       </c>
       <c r="C77" s="1"/>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>79</v>
       </c>
@@ -3049,7 +3058,7 @@
       </c>
       <c r="C78" s="1"/>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>80</v>
       </c>
@@ -3058,7 +3067,7 @@
       </c>
       <c r="C79" s="1"/>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>81</v>
       </c>
@@ -3067,7 +3076,7 @@
       </c>
       <c r="C80" s="1"/>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>82</v>
       </c>
@@ -3076,7 +3085,7 @@
       </c>
       <c r="C81" s="1"/>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>83</v>
       </c>
@@ -3085,7 +3094,7 @@
       </c>
       <c r="C82" s="1"/>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>84</v>
       </c>
@@ -3094,7 +3103,7 @@
       </c>
       <c r="C83" s="1"/>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>85</v>
       </c>
@@ -3103,7 +3112,7 @@
       </c>
       <c r="C84" s="1"/>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>86</v>
       </c>
@@ -3112,7 +3121,7 @@
       </c>
       <c r="C85" s="1"/>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>87</v>
       </c>
@@ -3121,7 +3130,7 @@
       </c>
       <c r="C86" s="1"/>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>88</v>
       </c>
@@ -3130,7 +3139,7 @@
       </c>
       <c r="C87" s="1"/>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>89</v>
       </c>
@@ -3139,7 +3148,7 @@
       </c>
       <c r="C88" s="1"/>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>91</v>
       </c>
@@ -3148,7 +3157,7 @@
       </c>
       <c r="C89" s="1"/>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>92</v>
       </c>
@@ -3157,7 +3166,7 @@
       </c>
       <c r="C90" s="1"/>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>93</v>
       </c>
@@ -3166,7 +3175,7 @@
       </c>
       <c r="C91" s="1"/>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>94</v>
       </c>
@@ -3175,7 +3184,7 @@
       </c>
       <c r="C92" s="1"/>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>95</v>
       </c>
@@ -3184,7 +3193,7 @@
       </c>
       <c r="C93" s="1"/>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>96</v>
       </c>
@@ -3193,7 +3202,7 @@
       </c>
       <c r="C94" s="1"/>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>97</v>
       </c>
@@ -3202,7 +3211,7 @@
       </c>
       <c r="C95" s="1"/>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>98</v>
       </c>
@@ -3211,7 +3220,7 @@
       </c>
       <c r="C96" s="1"/>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>99</v>
       </c>
@@ -3220,7 +3229,7 @@
       </c>
       <c r="C97" s="1"/>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>100</v>
       </c>
@@ -3229,7 +3238,7 @@
       </c>
       <c r="C98" s="1"/>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>101</v>
       </c>
@@ -3238,7 +3247,7 @@
       </c>
       <c r="C99" s="1"/>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>102</v>
       </c>
@@ -3247,7 +3256,7 @@
       </c>
       <c r="C100" s="1"/>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>103</v>
       </c>
@@ -3256,7 +3265,7 @@
       </c>
       <c r="C101" s="1"/>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>104</v>
       </c>
@@ -3265,7 +3274,7 @@
       </c>
       <c r="C102" s="1"/>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>105</v>
       </c>
@@ -3274,7 +3283,7 @@
       </c>
       <c r="C103" s="1"/>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>106</v>
       </c>
@@ -3283,7 +3292,7 @@
       </c>
       <c r="C104" s="1"/>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>107</v>
       </c>
@@ -3292,7 +3301,7 @@
       </c>
       <c r="C105" s="1"/>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>108</v>
       </c>
@@ -3301,7 +3310,7 @@
       </c>
       <c r="C106" s="1"/>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>109</v>
       </c>
@@ -3310,7 +3319,7 @@
       </c>
       <c r="C107" s="1"/>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>110</v>
       </c>
@@ -3319,7 +3328,7 @@
       </c>
       <c r="C108" s="1"/>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>111</v>
       </c>
@@ -3328,7 +3337,7 @@
       </c>
       <c r="C109" s="1"/>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>112</v>
       </c>
@@ -3337,7 +3346,7 @@
       </c>
       <c r="C110" s="1"/>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>113</v>
       </c>
@@ -3346,7 +3355,7 @@
       </c>
       <c r="C111" s="1"/>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>114</v>
       </c>
@@ -3355,7 +3364,7 @@
       </c>
       <c r="C112" s="1"/>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>115</v>
       </c>
@@ -3364,7 +3373,7 @@
       </c>
       <c r="C113" s="1"/>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>116</v>
       </c>
@@ -3373,7 +3382,7 @@
       </c>
       <c r="C114" s="1"/>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>117</v>
       </c>
@@ -3382,7 +3391,7 @@
       </c>
       <c r="C115" s="1"/>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>118</v>
       </c>
@@ -3391,7 +3400,7 @@
       </c>
       <c r="C116" s="1"/>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>119</v>
       </c>
@@ -3400,7 +3409,7 @@
       </c>
       <c r="C117" s="1"/>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>120</v>
       </c>
@@ -3409,7 +3418,7 @@
       </c>
       <c r="C118" s="1"/>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>121</v>
       </c>
@@ -3418,7 +3427,7 @@
       </c>
       <c r="C119" s="1"/>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>122</v>
       </c>
@@ -3427,7 +3436,7 @@
       </c>
       <c r="C120" s="1"/>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>123</v>
       </c>
@@ -3436,7 +3445,7 @@
       </c>
       <c r="C121" s="1"/>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>124</v>
       </c>
@@ -3445,7 +3454,7 @@
       </c>
       <c r="C122" s="1"/>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>125</v>
       </c>
@@ -3454,7 +3463,7 @@
       </c>
       <c r="C123" s="1"/>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>126</v>
       </c>
@@ -3463,7 +3472,7 @@
       </c>
       <c r="C124" s="1"/>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>127</v>
       </c>
@@ -3472,7 +3481,7 @@
       </c>
       <c r="C125" s="1"/>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>128</v>
       </c>
@@ -3481,7 +3490,7 @@
       </c>
       <c r="C126" s="1"/>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>129</v>
       </c>
@@ -3490,7 +3499,7 @@
       </c>
       <c r="C127" s="1"/>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>130</v>
       </c>
@@ -3499,7 +3508,7 @@
       </c>
       <c r="C128" s="1"/>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>131</v>
       </c>
@@ -3508,7 +3517,7 @@
       </c>
       <c r="C129" s="1"/>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>132</v>
       </c>
@@ -3517,7 +3526,7 @@
       </c>
       <c r="C130" s="1"/>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>133</v>
       </c>
@@ -3526,7 +3535,7 @@
       </c>
       <c r="C131" s="1"/>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>134</v>
       </c>
@@ -3535,7 +3544,7 @@
       </c>
       <c r="C132" s="1"/>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>135</v>
       </c>
@@ -3544,7 +3553,7 @@
       </c>
       <c r="C133" s="1"/>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>136</v>
       </c>
@@ -3553,7 +3562,7 @@
       </c>
       <c r="C134" s="1"/>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
         <v>137</v>
       </c>
@@ -3562,7 +3571,7 @@
       </c>
       <c r="C135" s="1"/>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>138</v>
       </c>
@@ -3571,7 +3580,7 @@
       </c>
       <c r="C136" s="1"/>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>139</v>
       </c>
@@ -3580,7 +3589,7 @@
       </c>
       <c r="C137" s="1"/>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
         <v>140</v>
       </c>
@@ -3589,7 +3598,7 @@
       </c>
       <c r="C138" s="1"/>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>141</v>
       </c>
@@ -3598,7 +3607,7 @@
       </c>
       <c r="C139" s="1"/>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>142</v>
       </c>
@@ -3607,7 +3616,7 @@
       </c>
       <c r="C140" s="1"/>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
         <v>143</v>
       </c>
@@ -3616,7 +3625,7 @@
       </c>
       <c r="C141" s="1"/>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>144</v>
       </c>
@@ -3625,7 +3634,7 @@
       </c>
       <c r="C142" s="1"/>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>145</v>
       </c>
@@ -3634,7 +3643,7 @@
       </c>
       <c r="C143" s="1"/>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>146</v>
       </c>
@@ -3643,7 +3652,7 @@
       </c>
       <c r="C144" s="1"/>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>147</v>
       </c>
@@ -3652,7 +3661,7 @@
       </c>
       <c r="C145" s="1"/>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>148</v>
       </c>
@@ -3661,7 +3670,7 @@
       </c>
       <c r="C146" s="1"/>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
         <v>149</v>
       </c>
@@ -3670,7 +3679,7 @@
       </c>
       <c r="C147" s="1"/>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>150</v>
       </c>
@@ -3679,7 +3688,7 @@
       </c>
       <c r="C148" s="1"/>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
         <v>151</v>
       </c>
@@ -3688,7 +3697,7 @@
       </c>
       <c r="C149" s="1"/>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>152</v>
       </c>
@@ -3697,7 +3706,7 @@
       </c>
       <c r="C150" s="1"/>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
         <v>153</v>
       </c>
@@ -3706,7 +3715,7 @@
       </c>
       <c r="C151" s="1"/>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
         <v>154</v>
       </c>
@@ -3715,7 +3724,7 @@
       </c>
       <c r="C152" s="1"/>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
         <v>155</v>
       </c>
@@ -3724,7 +3733,7 @@
       </c>
       <c r="C153" s="1"/>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>156</v>
       </c>
@@ -3733,7 +3742,7 @@
       </c>
       <c r="C154" s="1"/>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
         <v>157</v>
       </c>
@@ -3742,7 +3751,7 @@
       </c>
       <c r="C155" s="1"/>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>158</v>
       </c>
@@ -3751,7 +3760,7 @@
       </c>
       <c r="C156" s="1"/>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>159</v>
       </c>
@@ -3760,7 +3769,7 @@
       </c>
       <c r="C157" s="1"/>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>160</v>
       </c>
@@ -3769,7 +3778,7 @@
       </c>
       <c r="C158" s="1"/>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>161</v>
       </c>
@@ -3778,7 +3787,7 @@
       </c>
       <c r="C159" s="1"/>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>162</v>
       </c>
@@ -3787,7 +3796,7 @@
       </c>
       <c r="C160" s="1"/>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
         <v>163</v>
       </c>
@@ -3796,7 +3805,7 @@
       </c>
       <c r="C161" s="1"/>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>164</v>
       </c>
@@ -3805,7 +3814,7 @@
       </c>
       <c r="C162" s="1"/>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
         <v>165</v>
       </c>
@@ -3814,7 +3823,7 @@
       </c>
       <c r="C163" s="1"/>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
         <v>166</v>
       </c>
@@ -3823,7 +3832,7 @@
       </c>
       <c r="C164" s="1"/>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
         <v>167</v>
       </c>
@@ -3832,7 +3841,7 @@
       </c>
       <c r="C165" s="1"/>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
         <v>168</v>
       </c>
@@ -3841,7 +3850,7 @@
       </c>
       <c r="C166" s="1"/>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
         <v>238</v>
       </c>
@@ -3850,7 +3859,7 @@
       </c>
       <c r="C167" s="1"/>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>239</v>
       </c>
@@ -3858,7 +3867,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
         <v>240</v>
       </c>
@@ -3866,7 +3875,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
         <v>241</v>
       </c>
@@ -3874,7 +3883,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
         <v>242</v>
       </c>
@@ -3882,7 +3891,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
         <v>243</v>
       </c>
@@ -3890,7 +3899,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
         <v>169</v>
       </c>
@@ -3898,7 +3907,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
         <v>170</v>
       </c>
@@ -3906,7 +3915,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
         <v>171</v>
       </c>
@@ -3914,7 +3923,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
         <v>172</v>
       </c>
@@ -3922,7 +3931,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
         <v>90</v>
       </c>

</xml_diff>

<commit_message>
S4.US39 Consensus Default flag Web changes
</commit_message>
<xml_diff>
--- a/webapp/templates/GMIDSubmissionTemplate.xlsx
+++ b/webapp/templates/GMIDSubmissionTemplate.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\na20267\Desktop\BAM 2018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\na20267\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="5760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7455"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="658">
   <si>
     <t>Country</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Netting Default Flag</t>
   </si>
   <si>
-    <t>Market Default Flag</t>
-  </si>
-  <si>
     <t>Country Code</t>
   </si>
   <si>
@@ -684,12 +681,6 @@
     <t>Display</t>
   </si>
   <si>
-    <t>4 - Seeds</t>
-  </si>
-  <si>
-    <t>5 - Seasonal Spread w/o Disaggregation</t>
-  </si>
-  <si>
     <t>1 - Crop GMID</t>
   </si>
   <si>
@@ -1974,12 +1965,6 @@
     <t>WS - WESTERN SAMOA</t>
   </si>
   <si>
-    <t>XH</t>
-  </si>
-  <si>
-    <t>XH - XHRPTG CORPORATE R2</t>
-  </si>
-  <si>
     <t>XK - KOSOVO</t>
   </si>
   <si>
@@ -2023,6 +2008,39 @@
   </si>
   <si>
     <t xml:space="preserve">ZZ - UNKNOWN </t>
+  </si>
+  <si>
+    <t>Consensus Default Flag</t>
+  </si>
+  <si>
+    <t>0 - No Netting</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>MTO</t>
+  </si>
+  <si>
+    <t>0 - Active</t>
+  </si>
+  <si>
+    <t>0 - Do Not Exclude</t>
+  </si>
+  <si>
+    <t>1 - Sales Forecast(Units)</t>
+  </si>
+  <si>
+    <t>2 - Statistical Forecast(Units)</t>
+  </si>
+  <si>
+    <t>3 - Marketing Forecast(Units)</t>
+  </si>
+  <si>
+    <t>4 - Customer Forecast(Units)</t>
+  </si>
+  <si>
+    <t>5 - Charger</t>
   </si>
 </sst>
 </file>
@@ -2049,11 +2067,13 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -2076,7 +2096,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -2191,12 +2211,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2216,6 +2254,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2506,7 +2546,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2527,22 +2567,22 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>220</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>5</v>
+        <v>647</v>
       </c>
     </row>
   </sheetData>
@@ -2554,19 +2594,19 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B1048576">
       <formula1>Country</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D1048576">
       <formula1>Prod</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E1048576">
       <formula1>Netting</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H1048576">
       <formula1>Market</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F1048576">
       <formula1>Quadrant</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G1048576">
       <formula1>Channel</formula1>
     </dataValidation>
   </dataValidations>
@@ -2577,12 +2617,42 @@
   </headerFooter>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>DataSheet!B3:B282</xm:f>
+            <xm:f>DataSheet!B3:B281</xm:f>
           </x14:formula1>
           <xm:sqref>B2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>DataSheet!T3:T7</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>DataSheet!W3:W5</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>DataSheet!H3:H6</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>DataSheet!K3:K7</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>DataSheet!Q3:Q8</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2592,10 +2662,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W282"/>
+  <dimension ref="A1:W281"/>
   <sheetViews>
-    <sheetView topLeftCell="A276" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView topLeftCell="A259" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A267" sqref="A267:XFD267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2619,2728 +2689,2772 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="D1" s="18" t="s">
+      <c r="B1" s="20"/>
+      <c r="D1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="18"/>
-      <c r="G1" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="18"/>
-      <c r="J1" s="18" t="s">
+      <c r="E1" s="20"/>
+      <c r="G1" s="20" t="s">
+        <v>647</v>
+      </c>
+      <c r="H1" s="20"/>
+      <c r="J1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="18"/>
-      <c r="M1" s="18" t="s">
-        <v>213</v>
-      </c>
-      <c r="N1" s="18"/>
-      <c r="P1" s="18" t="s">
+      <c r="K1" s="20"/>
+      <c r="M1" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="N1" s="20"/>
+      <c r="P1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="18"/>
-      <c r="S1" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="T1" s="17"/>
-      <c r="V1" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="W1" s="18"/>
+      <c r="Q1" s="20"/>
+      <c r="S1" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="T1" s="19"/>
+      <c r="V1" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="W1" s="20"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>7</v>
-      </c>
       <c r="D2" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>174</v>
-      </c>
       <c r="G2" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="H2" s="7" t="s">
-        <v>204</v>
-      </c>
       <c r="J2" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="K2" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="K2" s="7" t="s">
-        <v>204</v>
-      </c>
       <c r="M2" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="N2" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="N2" s="7" t="s">
-        <v>204</v>
-      </c>
       <c r="P2" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q2" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="Q2" s="7" t="s">
-        <v>204</v>
-      </c>
       <c r="S2" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="T2" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="T2" s="7" t="s">
-        <v>204</v>
-      </c>
       <c r="V2" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="W2" s="7" t="s">
         <v>203</v>
-      </c>
-      <c r="W2" s="7" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="G3" s="13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>205</v>
-      </c>
-      <c r="J3" s="10">
-        <v>1</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="M3" s="10">
-        <v>1</v>
-      </c>
-      <c r="N3" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="P3" s="10">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="S3" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="T3" s="11" t="s">
-        <v>221</v>
-      </c>
-      <c r="W3" t="s">
-        <v>226</v>
+        <v>653</v>
+      </c>
+      <c r="J3" s="8">
+        <v>0</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>648</v>
+      </c>
+      <c r="M3" s="8">
+        <v>0</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>652</v>
+      </c>
+      <c r="P3" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="9" t="s">
+        <v>651</v>
+      </c>
+      <c r="S3" s="8" t="s">
+        <v>649</v>
+      </c>
+      <c r="T3" s="9" t="s">
+        <v>649</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>650</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="G4" s="14">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="J4" s="8">
-        <v>2</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="M4" s="8">
-        <v>2</v>
-      </c>
-      <c r="N4" s="9" t="s">
+        <v>654</v>
+      </c>
+      <c r="J4" s="10">
+        <v>1</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="M4" s="10">
+        <v>1</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="P4" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="P4" s="8">
-        <v>2</v>
-      </c>
-      <c r="Q4" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="S4" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="T4" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>225</v>
+      <c r="S4" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="T4" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>230</v>
-      </c>
-      <c r="J5" s="4">
+        <v>227</v>
+      </c>
+      <c r="G5">
         <v>3</v>
       </c>
-      <c r="K5" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="M5" s="4">
-        <v>3</v>
-      </c>
-      <c r="N5" s="5" t="s">
+      <c r="H5" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="J5" s="8">
+        <v>2</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="M5" s="8">
+        <v>2</v>
+      </c>
+      <c r="N5" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="P5" s="8">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="P5" s="4">
-        <v>3</v>
-      </c>
-      <c r="Q5" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="S5" s="10" t="s">
-        <v>223</v>
-      </c>
-      <c r="T5" s="11" t="s">
-        <v>223</v>
+      <c r="S5" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="T5" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>231</v>
-      </c>
-      <c r="J6" s="8">
-        <v>5</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>256</v>
-      </c>
-      <c r="P6" s="8">
+        <v>228</v>
+      </c>
+      <c r="G6">
         <v>4</v>
       </c>
-      <c r="Q6" s="9" t="s">
-        <v>257</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="T6" s="3" t="s">
-        <v>225</v>
+      <c r="H6" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="J6" s="4">
+        <v>3</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="M6" s="4">
+        <v>3</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="P6" s="4">
+        <v>3</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="S6" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="T6" s="11" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>232</v>
-      </c>
-      <c r="K7" s="1"/>
+        <v>229</v>
+      </c>
+      <c r="J7" s="8">
+        <v>5</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="P7" s="8">
+        <v>4</v>
+      </c>
+      <c r="Q7" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>233</v>
+        <v>230</v>
+      </c>
+      <c r="P8" s="17">
+        <v>5</v>
+      </c>
+      <c r="Q8" s="18" t="s">
+        <v>657</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="15" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="15" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="15" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C31" s="1"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="C32" s="1"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C33" s="1"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="C34" s="1"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="C35" s="1"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="C36" s="1"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="C37" s="1"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="C38" s="1"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="C39" s="1"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C40" s="1"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="C41" s="1"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C42" s="1"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="C43" s="1"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C44" s="1"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C45" s="1"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C46" s="1"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="C47" s="1"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="C48" s="1"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="C49" s="1"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="C50" s="1"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="C51" s="1"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="C52" s="1"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="16" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B53" s="16" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="C53" s="1"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="16" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="C54" s="1"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="16" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C55" s="1"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="16" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="C56" s="1"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="C57" s="1"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B58" s="16" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C58" s="1"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="16" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="C59" s="1"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="16" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="C60" s="1"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="16" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="C61" s="1"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="C62" s="1"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B63" s="16" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="C63" s="1"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C64" s="1"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="16" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C65" s="1"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B66" s="16" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C66" s="1"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B67" s="16" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="C67" s="1"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B68" s="16" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="C68" s="1"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B69" s="16" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="C69" s="1"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B70" s="16" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="C70" s="1"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="16" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B71" s="16" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="C71" s="1"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="16" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B72" s="16" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="C72" s="1"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B73" s="16" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="C73" s="1"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B74" s="16" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C74" s="1"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B75" s="16" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="C75" s="1"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="16" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B76" s="16" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="C76" s="1"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B77" s="16" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C77" s="1"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="16" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B78" s="16" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="C78" s="1"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="16" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B79" s="16" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="C79" s="1"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B80" s="16" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="C80" s="1"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="16" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B81" s="16" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="C81" s="1"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="16" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B82" s="16" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="C82" s="1"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="16" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B83" s="16" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="C83" s="1"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="16" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B84" s="16" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="C84" s="1"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B85" s="16" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C85" s="1"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B86" s="16" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="C86" s="1"/>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="16" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B87" s="16" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="C87" s="1"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B88" s="16" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="C88" s="1"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B89" s="16" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="C89" s="1"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B90" s="16" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="C90" s="1"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="16" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B91" s="16" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="C91" s="1"/>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="16" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B92" s="16" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="C92" s="1"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B93" s="16" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="C93" s="1"/>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B94" s="16" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="C94" s="1"/>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B95" s="16" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="C95" s="1"/>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="16" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B96" s="16" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="C96" s="1"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B97" s="16" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="C97" s="1"/>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B98" s="16" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="C98" s="1"/>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B99" s="16" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="C99" s="1"/>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="16" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B100" s="16" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="C100" s="1"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="16" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B101" s="16" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="C101" s="1"/>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B102" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="C102" s="1"/>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="16" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B103" s="16" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C103" s="1"/>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B104" s="16" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="C104" s="1"/>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B105" s="16" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="C105" s="1"/>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B106" s="16" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="C106" s="1"/>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B107" s="16" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="C107" s="1"/>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="16" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B108" s="16" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="C108" s="1"/>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B109" s="16" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="C109" s="1"/>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B110" s="16" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="C110" s="1"/>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B111" s="16" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="C111" s="1"/>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B112" s="16" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="C112" s="1"/>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="16" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B113" s="16" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="C113" s="1"/>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B114" s="16" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="C114" s="1"/>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B115" s="16" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="C115" s="1"/>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B116" s="16" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="C116" s="1"/>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B117" s="16" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="C117" s="1"/>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B118" s="16" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C118" s="1"/>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B119" s="16" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="C119" s="1"/>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B120" s="16" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="C120" s="1"/>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B121" s="16" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="C121" s="1"/>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B122" s="16" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="C122" s="1"/>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="16" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B123" s="16" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="C123" s="1"/>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="16" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B124" s="16" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="C124" s="1"/>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="16" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B125" s="16" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="C125" s="1"/>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="16" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B126" s="16" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="C126" s="1"/>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="16" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B127" s="16" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="C127" s="1"/>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B128" s="16" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="C128" s="1"/>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B129" s="16" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="C129" s="1"/>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B130" s="16" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="C130" s="1"/>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B131" s="16" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="C131" s="1"/>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="16" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B132" s="16" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="C132" s="1"/>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B133" s="16" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="C133" s="1"/>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="16" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B134" s="16" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="C134" s="1"/>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B135" s="16" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="C135" s="1"/>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B136" s="16" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="C136" s="1"/>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B137" s="16" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C137" s="1"/>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="16" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B138" s="16" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C138" s="1"/>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B139" s="16" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="C139" s="1"/>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B140" s="16" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="C140" s="1"/>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B141" s="16" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="C141" s="1"/>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B142" s="16" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="C142" s="1"/>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B143" s="16" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="C143" s="1"/>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="16" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B144" s="16" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="C144" s="1"/>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B145" s="16" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="C145" s="1"/>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="16" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B146" s="16" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="C146" s="1"/>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B147" s="16" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="C147" s="1"/>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="16" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B148" s="16" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="C148" s="1"/>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B149" s="16" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="C149" s="1"/>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B150" s="16" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="C150" s="1"/>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B151" s="16" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="C151" s="1"/>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B152" s="16" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="C152" s="1"/>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B153" s="16" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="C153" s="1"/>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="16" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B154" s="16" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="C154" s="1"/>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B155" s="16" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="C155" s="1"/>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B156" s="16" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="C156" s="1"/>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="16" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B157" s="16" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="C157" s="1"/>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B158" s="16" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="C158" s="1"/>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B159" s="16" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="C159" s="1"/>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="16" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B160" s="16" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="C160" s="1"/>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B161" s="16" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="C161" s="1"/>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B162" s="16" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="C162" s="1"/>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B163" s="16" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="C163" s="1"/>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B164" s="16" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="C164" s="1"/>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B165" s="16" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="C165" s="1"/>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B166" s="16" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="C166" s="1"/>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B167" s="16" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="16" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B168" s="16" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B169" s="16" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B170" s="16" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B171" s="16" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B172" s="16" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B173" s="16" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="16" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B174" s="16" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="16" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B175" s="16" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B176" s="16" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B177" s="16" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B178" s="16" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B179" s="16" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B180" s="16" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B181" s="16" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B182" s="16" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="16" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B183" s="16" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B184" s="16" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B185" s="16" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="16" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B186" s="16" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="16" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B187" s="16" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B188" s="16" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="16" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B189" s="16" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B190" s="16" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="16" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B191" s="16" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B192" s="16" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B193" s="16" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="16" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B194" s="16" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="16" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B195" s="16" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="16" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B196" s="16" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="16" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B197" s="16" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B198" s="16" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B199" s="16" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B200" s="16" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" s="16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B201" s="16" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" s="16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B202" s="16" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B203" s="16" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" s="16" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B204" s="16" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B205" s="16" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B206" s="16" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B207" s="16" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B208" s="16" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B209" s="16" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B210" s="16" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B211" s="16" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B212" s="16" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" s="16" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B213" s="16" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B214" s="16" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" s="16" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B215" s="16" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" s="16" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B216" s="16" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B217" s="16" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" s="16" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B218" s="16" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B219" s="16" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" s="16" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B220" s="16" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B221" s="16" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B222" s="16" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" s="16" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B223" s="16" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B224" s="16" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" s="16" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B225" s="16" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" s="16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B226" s="16" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B227" s="16" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B228" s="16" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" s="16" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B229" s="16" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" s="16" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B230" s="16" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" s="16" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B231" s="16" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B232" s="16" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" s="16" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B233" s="16" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B234" s="16" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B235" s="16" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" s="16" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B236" s="16" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" s="16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B237" s="16" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" s="16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B238" s="16" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" s="16" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B239" s="16" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" s="16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B240" s="16" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" s="16" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B241" s="16" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" s="16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B242" s="16" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" s="16" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="B243" s="16" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" s="16" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B244" s="16" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" s="16" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="B245" s="16" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" s="16" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B246" s="16" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" s="16" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B247" s="16" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" s="16" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B248" s="16" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" s="16" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B249" s="16" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" s="16" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B250" s="16" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" s="16" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="B251" s="16" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" s="16" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="B252" s="16" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" s="16" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B253" s="16" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" s="16" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B254" s="16" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" s="16" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="B255" s="16" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" s="16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B256" s="16" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B257" s="16" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" s="16" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B258" s="16" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" s="16" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B259" s="16" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B260" s="16" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" s="16" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B261" s="16" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" s="16" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="B262" s="16" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" s="16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B263" s="16" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" s="16" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B264" s="16" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" s="16" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="B265" s="16" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" s="16" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="B266" s="16" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" s="16" t="s">
-        <v>635</v>
+        <v>358</v>
       </c>
       <c r="B267" s="16" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" s="16" t="s">
-        <v>361</v>
+        <v>224</v>
       </c>
       <c r="B268" s="16" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" s="16" t="s">
-        <v>227</v>
+        <v>168</v>
       </c>
       <c r="B269" s="16" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" s="16" t="s">
-        <v>169</v>
+        <v>359</v>
       </c>
       <c r="B270" s="16" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" s="16" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B271" s="16" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" s="16" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B272" s="16" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" s="16" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B273" s="16" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" s="16" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B274" s="16" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" s="16" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B275" s="16" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" s="16" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B276" s="16" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" s="16" t="s">
-        <v>368</v>
+        <v>169</v>
       </c>
       <c r="B277" s="16" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
@@ -5348,39 +5462,31 @@
         <v>170</v>
       </c>
       <c r="B278" s="16" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" s="16" t="s">
-        <v>171</v>
+        <v>366</v>
       </c>
       <c r="B279" s="16" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280" s="16" t="s">
-        <v>369</v>
+        <v>171</v>
       </c>
       <c r="B280" s="16" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281" s="16" t="s">
-        <v>172</v>
+        <v>367</v>
       </c>
       <c r="B281" s="16" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A282" s="16" t="s">
-        <v>370</v>
-      </c>
-      <c r="B282" s="16" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
     </row>
   </sheetData>

</xml_diff>